<commit_message>
added el. smd cap and dac
</commit_message>
<xml_diff>
--- a/library/power_supplies.xlsx
+++ b/library/power_supplies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitProjects\elem_altium_db2\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6705D7F-2284-4C6A-962B-1C769D3B1AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B3B457-4381-494E-9031-F18CEBC77A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{EE2E7F00-6B54-4C0B-98D7-835E87062BAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{EE2E7F00-6B54-4C0B-98D7-835E87062BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="ac-dc" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="186">
   <si>
     <t>Part Number</t>
   </si>
@@ -575,13 +575,57 @@
   </si>
   <si>
     <t>TPS54360</t>
+  </si>
+  <si>
+    <t>ONSEMI</t>
+  </si>
+  <si>
+    <r>
+      <t>LP2951</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inter"/>
+      </rPr>
+      <t>ACDG</t>
+    </r>
+  </si>
+  <si>
+    <t>LP2951</t>
+  </si>
+  <si>
+    <t>TPL740ADJ-5TR SOT23-5</t>
+  </si>
+  <si>
+    <t>LMC7660</t>
+  </si>
+  <si>
+    <r>
+      <t>LMC7660</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inter"/>
+      </rPr>
+      <t>IM 8-SOIC</t>
+    </r>
+  </si>
+  <si>
+    <t>LMC7660IM</t>
+  </si>
+  <si>
+    <t>LP2951ACDG 8-SOIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -596,6 +640,11 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Inter"/>
     </font>
   </fonts>
   <fills count="3">
@@ -625,13 +674,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent 3 2" xfId="1" xr:uid="{07D6D35A-A25D-4183-ACA2-756DA14CBAEA}"/>
@@ -953,12 +1003,12 @@
       <selection activeCell="A3" sqref="A3:XFD36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -984,7 +1034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1020,7 +1070,7 @@
       <selection activeCell="A7" sqref="A7:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
@@ -1029,7 +1079,7 @@
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1078,7 +1128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1101,7 +1151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1124,7 +1174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1147,7 +1197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1177,13 +1227,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4D8C3D-D832-496B-AB92-259D2AD291EC}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD36"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -1194,7 +1244,7 @@
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>145</v>
       </c>
@@ -1243,7 +1293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>148</v>
       </c>
@@ -1266,7 +1316,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>152</v>
       </c>
@@ -1289,7 +1339,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>157</v>
       </c>
@@ -1312,7 +1362,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>159</v>
       </c>
@@ -1335,7 +1385,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>164</v>
       </c>
@@ -1358,7 +1408,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>167</v>
       </c>
@@ -1381,7 +1431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>171</v>
       </c>
@@ -1404,7 +1454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>175</v>
       </c>
@@ -1424,6 +1474,29 @@
         <v>172</v>
       </c>
       <c r="G10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1440,7 +1513,7 @@
       <selection activeCell="A5" sqref="A5:XFD38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
@@ -1449,7 +1522,7 @@
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1475,7 +1548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -1498,7 +1571,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>138</v>
       </c>
@@ -1521,7 +1594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -1551,13 +1624,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36817BF-F161-418A-9B8F-87A18459EBCD}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
@@ -1567,7 +1640,7 @@
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1616,7 +1689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1639,7 +1712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1662,7 +1735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1685,7 +1758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1708,7 +1781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1731,7 +1804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1754,7 +1827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1777,7 +1850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -1800,7 +1873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -1823,7 +1896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1846,7 +1919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1869,7 +1942,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1892,7 +1965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1915,7 +1988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -1938,7 +2011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1961,7 +2034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1984,7 +2057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -2007,7 +2080,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -2030,7 +2103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -2053,7 +2126,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -2076,7 +2149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -2099,7 +2172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>86</v>
       </c>
@@ -2122,7 +2195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -2145,7 +2218,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>92</v>
       </c>
@@ -2168,7 +2241,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -2191,7 +2264,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>96</v>
       </c>
@@ -2214,7 +2287,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>98</v>
       </c>
@@ -2237,7 +2310,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -2245,7 +2318,7 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>181</v>
       </c>
       <c r="D30" t="s">
         <v>100</v>
@@ -2258,6 +2331,29 @@
       </c>
       <c r="G30" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E31" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2273,7 +2369,7 @@
       <selection activeCell="A4" sqref="A4:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
@@ -2283,7 +2379,7 @@
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2309,7 +2405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -2329,7 +2425,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>103</v>
       </c>
@@ -2365,14 +2461,14 @@
       <selection activeCell="A6" sqref="A6:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2398,7 +2494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -2421,7 +2517,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>113</v>
       </c>
@@ -2444,7 +2540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -2467,7 +2563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -2499,11 +2595,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE80AA7D-5B01-4429-B668-37BD5F31C3F5}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
@@ -2512,7 +2608,7 @@
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2538,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>125</v>
       </c>
@@ -2562,7 +2658,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>128</v>
       </c>
@@ -2586,7 +2682,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>131</v>
       </c>

</xml_diff>